<commit_message>
ESS. Relaxation slacks. Test
</commit_message>
<xml_diff>
--- a/data/CS6/Market Data/CS6_market_data_2025.xlsx
+++ b/data/CS6/Market Data/CS6_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS6\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857825D0-0283-4476-9CD6-3DE0D6F4CC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA30090-7979-44B3-A9EC-0AA3977A0017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34320" yWindow="-10620" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. Branch limit on current.
</commit_message>
<xml_diff>
--- a/data/CS6/Market Data/CS6_market_data_2025.xlsx
+++ b/data/CS6/Market Data/CS6_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS6\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8356109A-0387-4664-8F2D-2C15D30BA481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EAA3AF-9D52-471B-9F76-AA35920D21F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33450" yWindow="-11490" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33885" yWindow="-11055" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>